<commit_message>
gaze preference in time script updated
</commit_message>
<xml_diff>
--- a/data/DatasetsLabels.xlsx
+++ b/data/DatasetsLabels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pradyumna/Documents/GiTs/Sepulveda_et_al_2020/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D93BB73-E268-6D4F-A8EF-FD4ECD30608B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F8AABD-F266-EE4A-A1C8-EB69D2F6F183}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25740" yWindow="21720" windowWidth="26840" windowHeight="15940" xr2:uid="{458455FA-77E4-3A41-918D-8E92563619C8}"/>
+    <workbookView xWindow="31000" yWindow="13600" windowWidth="26840" windowHeight="15940" xr2:uid="{458455FA-77E4-3A41-918D-8E92563619C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Value" sheetId="1" r:id="rId1"/>
@@ -307,9 +307,6 @@
     <t>right item confidence in the familiarity reported in BDM bid</t>
   </si>
   <si>
-    <t>z-scored measures of varaibles stated above</t>
-  </si>
-  <si>
     <t>z-scored trial gaze shift frequency</t>
   </si>
   <si>
@@ -467,6 +464,9 @@
   </si>
   <si>
     <t>DataPerceptualFramingNotebooks</t>
+  </si>
+  <si>
+    <t>z-scored measures of variables stated above</t>
   </si>
 </sst>
 </file>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2B7FC3C-E81F-EE44-9190-D144E33A1470}">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -849,7 +849,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -913,7 +913,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1105,7 +1105,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -1113,7 +1113,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1145,7 +1145,7 @@
         <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -1153,7 +1153,7 @@
         <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -1161,7 +1161,7 @@
         <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -1169,7 +1169,7 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -1185,7 +1185,7 @@
         <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -1193,7 +1193,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -1201,7 +1201,7 @@
         <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -1209,7 +1209,7 @@
         <v>40</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -1217,7 +1217,7 @@
         <v>41</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -1225,7 +1225,7 @@
         <v>42</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1233,7 +1233,7 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -1241,7 +1241,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1249,7 +1249,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1257,7 +1257,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1265,7 +1265,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1273,7 +1273,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1281,7 +1281,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1289,7 +1289,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -1297,7 +1297,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1305,7 +1305,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1313,7 +1313,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1321,25 +1321,25 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B66" t="s">
         <v>60</v>
@@ -1347,44 +1347,44 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B67" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B68" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B74" t="s">
         <v>59</v>
@@ -1392,7 +1392,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B75" t="s">
         <v>60</v>
@@ -1400,23 +1400,23 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B76" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B78" t="s">
         <v>63</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B79" t="s">
         <v>65</v>
@@ -1432,18 +1432,18 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B80" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B81" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1463,7 +1463,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1487,7 +1487,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1495,7 +1495,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1503,7 +1503,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1511,7 +1511,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1543,7 +1543,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1647,7 +1647,7 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1655,7 +1655,7 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1663,7 +1663,7 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -1671,7 +1671,7 @@
         <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -1679,7 +1679,7 @@
         <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -1687,7 +1687,7 @@
         <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -1695,7 +1695,7 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -1703,7 +1703,7 @@
         <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -1711,23 +1711,23 @@
         <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -1735,7 +1735,7 @@
         <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -1743,7 +1743,7 @@
         <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -1751,70 +1751,70 @@
         <v>58</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B53" t="s">
         <v>59</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B54" t="s">
         <v>60</v>
@@ -1830,50 +1830,50 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>